<commit_message>
Se agrega columna en reporte de locales en excel
</commit_message>
<xml_diff>
--- a/static/docs/reporte_locales.xlsx
+++ b/static/docs/reporte_locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\web\feria\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCB4143-ACA4-4FC0-984E-7823B6C2AB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF90D2-6D0E-4529-9479-00C41950403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0401FBD8-E136-49A6-ACF6-5EB4423BA7C8}"/>
+    <workbookView xWindow="-24120" yWindow="1245" windowWidth="24240" windowHeight="13020" xr2:uid="{0401FBD8-E136-49A6-ACF6-5EB4423BA7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCALES" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Stand</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Giro</t>
+  </si>
+  <si>
+    <t>Método de Asignación</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5B52A7-C81D-4B89-840E-6107D4E4A925}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,9 +485,10 @@
     <col min="7" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="20.88671875" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -497,8 +501,9 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,11 +533,14 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>